<commit_message>
created dictionary and fixed pyplot ssue not being reset between MLR and Kmenas
</commit_message>
<xml_diff>
--- a/results/ML/MLR_cEnroll_nPSU_nS1S2_vs_Desertor/evaluateRegModel.xlsx
+++ b/results/ML/MLR_cEnroll_nPSU_nS1S2_vs_Desertor/evaluateRegModel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Reference\models\desertorstudent\results\ML\MLR_cEnroll_nPSU_nS1S2_vs_Desertor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reference\models\desertorstudent\results\ML\MLR_cEnroll_nPSU_nS1S2_vs_Desertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC99B367-57E7-411F-8475-AE3549FE1098}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33992D23-5BED-4B5C-A420-91595DC7A5BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16800" yWindow="0" windowWidth="12000" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <t>x</t>
   </si>
   <si>
-    <t>S1_GRD_4TO49, S1_GRD_5TO59, S2_GRD_3TO39, S2_GRD_4TO49, S2_GRD_5TO59, S2_BEST_GRD, SchoolRegion_1, SchoolType_4, Campus_1, PostulationType_1</t>
+    <t>LangScr, S1_DRP, S1_GRD_1TO19, S1_GRD_4TO49, S1_GRD_5TO59, S2_GRD_1TO19, S2_GRD_3TO39, S2_GRD_4TO49, S2_GRD_5TO59, S2_GRD_6TO7, S2_VS_S1, SchoolRegion_1, SchoolRegion_2, SchoolRegion_3, SchoolType_2, MotherEd_7, Campus_1, PostulationType_1</t>
   </si>
   <si>
     <t>y</t>
@@ -444,7 +444,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="145.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="248.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -477,7 +477,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>0.79629629629629628</v>
+        <v>0.77777777777777779</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -493,7 +493,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>0.83333333333333337</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -501,7 +501,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>0.85526315789473695</v>
+        <v>0.8441558441558441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>